<commit_message>
added file to preprocess data for regression analysis
</commit_message>
<xml_diff>
--- a/Backend/Model Metrics/best_params_rfc_vent.xlsx
+++ b/Backend/Model Metrics/best_params_rfc_vent.xlsx
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>